<commit_message>
Deploying to gh-pages from  @ 5536ae34108f994a6c198d16aa54c2468cd9f62d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.7.1.xlsx
+++ b/en/downloads/data-excel/3.7.1.xlsx
@@ -118,15 +118,9 @@
     <t>3.7.1 Proportion of women of reproductive age (aged 15–49 years) who have their need for family planning satisfied with modern methods</t>
   </si>
   <si>
-    <t>3.7.1. Доля женщин репродуктивного возраста (от 15 до 49 лет), чьи потребности по планированию семьи удовлетворяются современными методами</t>
-  </si>
-  <si>
     <t>(в процентах)</t>
   </si>
   <si>
-    <t>(per cents)</t>
-  </si>
-  <si>
     <t>20-24</t>
   </si>
   <si>
@@ -335,6 +329,12 @@
   </si>
   <si>
     <t xml:space="preserve">3.7.1 Үй-бүлөнү пландаштыруу боюнча муктаждыктары заманбап ыкмалар менен канааттандырылган репродуктивдүү жаш курактагы (15 жаштан 49 жашка чейинки) аялдардын үлүшү </t>
+  </si>
+  <si>
+    <t>3.7.1 Доля женщин репродуктивного возраста (от 15 до 49 лет), чьи потребности по планированию семьи удовлетворяются современными методами</t>
+  </si>
+  <si>
+    <t>(in per cents)</t>
   </si>
 </sst>
 </file>
@@ -344,7 +344,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _р_._-;\-* #,##0.00\ _р_._-;_-* &quot;-&quot;??\ _р_._-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -656,36 +656,36 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1024,10 +1024,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="63.75">
       <c r="A1" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>33</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="1"/>
@@ -1244,26 +1244,26 @@
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1">
       <c r="A15" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="38"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="34">
         <v>43.1</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="34">
         <v>41.4</v>
@@ -1291,26 +1291,26 @@
     </row>
     <row r="18" spans="1:5" s="24" customFormat="1">
       <c r="A18" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="40"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="35">
         <v>17.399999999999999</v>
@@ -1321,13 +1321,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="35">
         <v>28.9</v>
@@ -1338,13 +1338,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="35">
         <v>39.200000000000003</v>
@@ -1355,13 +1355,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="35">
         <v>50.4</v>
@@ -1372,13 +1372,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" s="35">
         <v>57.2</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="35">
         <v>52.2</v>
@@ -1406,13 +1406,13 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" s="35">
         <v>29.3</v>
@@ -1423,43 +1423,43 @@
     </row>
     <row r="26" spans="1:5" s="24" customFormat="1">
       <c r="A26" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D27" s="34">
         <v>20.399999999999999</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" s="34">
         <v>36.5</v>
@@ -1470,13 +1470,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="34">
         <v>42.1</v>
@@ -1487,13 +1487,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" s="34">
         <v>43.3</v>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D31" s="34">
         <v>43.7</v>
@@ -1521,26 +1521,26 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>102</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="34">
@@ -1549,13 +1549,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="D34" s="34"/>
       <c r="E34" s="34">
@@ -1564,26 +1564,26 @@
     </row>
     <row r="35" spans="1:5" s="24" customFormat="1">
       <c r="A35" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="39"/>
       <c r="E35" s="42"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D36" s="34">
         <v>42.5</v>
@@ -1594,13 +1594,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D37" s="34">
         <v>37.799999999999997</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D38" s="34">
         <v>39.1</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="34">
         <v>45.1</v>
@@ -1645,13 +1645,13 @@
     </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1">
       <c r="A40" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D40" s="43">
         <v>45.3</v>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="41" spans="1:5" ht="24">
       <c r="A41" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="20" t="s">
         <v>47</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="D41" s="20"/>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 4817e3b5c322d1c11af5fbfb3030f828eab3b658 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.7.1.xlsx
+++ b/en/downloads/data-excel/3.7.1.xlsx
@@ -316,9 +316,6 @@
     <t>3.7.1 Доля женщин репродуктивного возраста (от 15 до 49 лет), чьи потребности по планированию семьи удовлетворяются современными методами</t>
   </si>
   <si>
-    <t>(in per cents)</t>
-  </si>
-  <si>
     <t>(43,5)</t>
   </si>
   <si>
@@ -337,9 +334,6 @@
     <t>По данным кластерного обследования по многим показателям, 2014г., 2018г., 2023г.</t>
   </si>
   <si>
-    <t>According to the cluster survey in many respects, 2014, 2018, 2023</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -350,6 +344,12 @@
   </si>
   <si>
     <t>Age, years old</t>
+  </si>
+  <si>
+    <t>(in per cent)</t>
+  </si>
+  <si>
+    <t>According to the Multiple Indicator Cluster Survey, 2014, 2018, 2023</t>
   </si>
 </sst>
 </file>
@@ -361,7 +361,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _р_._-;\-* #,##0.00\ _р_._-;_-* &quot;-&quot;??\ _р_._-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +525,13 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -660,9 +667,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,6 +738,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1081,16 +1088,16 @@
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="22"/>
+      <c r="C2" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="21"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1">
@@ -1110,7 +1117,7 @@
       <c r="C4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>2014</v>
       </c>
       <c r="E4" s="3">
@@ -1130,29 +1137,29 @@
       <c r="C5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>42</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>67.400000000000006</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="C6" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
@@ -1164,13 +1171,13 @@
       <c r="C7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>45</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="34">
         <v>48.6</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="34">
         <v>43.3</v>
       </c>
     </row>
@@ -1184,13 +1191,13 @@
       <c r="C8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <v>31.4</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="34">
         <v>56.2</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="34">
         <v>51.5</v>
       </c>
     </row>
@@ -1204,13 +1211,13 @@
       <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="35">
         <v>46</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="34">
         <v>65.099999999999994</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <v>61.9</v>
       </c>
     </row>
@@ -1224,13 +1231,13 @@
       <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="35">
         <v>58.9</v>
       </c>
-      <c r="E10" s="35">
+      <c r="E10" s="34">
         <v>79.8</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="34">
         <v>74</v>
       </c>
     </row>
@@ -1244,13 +1251,13 @@
       <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="35">
         <v>38.4</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="34">
         <v>71.099999999999994</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="34">
         <v>56</v>
       </c>
     </row>
@@ -1264,13 +1271,13 @@
       <c r="C12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="35">
         <v>43.4</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="34">
         <v>79.099999999999994</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="34">
         <v>80.900000000000006</v>
       </c>
     </row>
@@ -1284,13 +1291,13 @@
       <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="35">
         <v>47.8</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="34">
         <v>70.7</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="34">
         <v>61.3</v>
       </c>
     </row>
@@ -1304,13 +1311,13 @@
       <c r="C14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <v>47</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="34">
         <v>69.599999999999994</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="34">
         <v>71.8</v>
       </c>
     </row>
@@ -1324,32 +1331,32 @@
       <c r="C15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="33">
         <v>38.299999999999997</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="34">
         <v>71.3</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="34">
         <v>58.6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="24" customFormat="1">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:6" s="23" customFormat="1">
+      <c r="A16" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1358,18 +1365,18 @@
       <c r="C17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="33">
         <v>43.1</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="34">
         <v>68.599999999999994</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="34">
         <v>60.6</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1378,32 +1385,32 @@
       <c r="C18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="33">
         <v>41.4</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="34">
         <v>66.7</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="34">
         <v>58.3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="24" customFormat="1">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:6" s="23" customFormat="1">
+      <c r="A19" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -1412,13 +1419,13 @@
       <c r="C20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="35">
+      <c r="D20" s="34">
         <v>17.399999999999999</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="34">
         <v>31.7</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1432,13 +1439,13 @@
       <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="35">
+      <c r="D21" s="34">
         <v>28.9</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="34">
         <v>53.8</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="34">
         <v>35.700000000000003</v>
       </c>
     </row>
@@ -1452,13 +1459,13 @@
       <c r="C22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="34">
         <v>39.200000000000003</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="34">
         <v>59.9</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="34">
         <v>50.1</v>
       </c>
     </row>
@@ -1472,13 +1479,13 @@
       <c r="C23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="34">
         <v>50.4</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="34">
         <v>76.2</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="34">
         <v>57</v>
       </c>
     </row>
@@ -1492,13 +1499,13 @@
       <c r="C24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="34">
         <v>57.2</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="34">
         <v>74.5</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="34">
         <v>66.3</v>
       </c>
     </row>
@@ -1512,13 +1519,13 @@
       <c r="C25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="34">
         <v>52.2</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="34">
         <v>68.7</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="34">
         <v>68.900000000000006</v>
       </c>
     </row>
@@ -1532,32 +1539,32 @@
       <c r="C26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="34">
         <v>29.3</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="34">
         <v>66</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="34">
         <v>63.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="24" customFormat="1">
-      <c r="A27" s="26" t="s">
+    <row r="27" spans="1:6" s="23" customFormat="1">
+      <c r="A27" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -1566,18 +1573,18 @@
       <c r="C28" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="33">
         <v>20.399999999999999</v>
       </c>
-      <c r="E28" s="41" t="s">
+      <c r="E28" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="41" t="s">
+      <c r="F28" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -1586,18 +1593,18 @@
       <c r="C29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="33">
         <v>36.5</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="33">
         <v>67.8</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="33">
         <v>62.9</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -1606,18 +1613,18 @@
       <c r="C30" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="33">
         <v>42.1</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="33">
         <v>62.9</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="33">
         <v>55.8</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>79</v>
       </c>
       <c r="B31" s="18" t="s">
@@ -1626,18 +1633,18 @@
       <c r="C31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="33">
         <v>43.3</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E31" s="33">
         <v>66.2</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="33">
         <v>55.2</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B32" s="18" t="s">
@@ -1646,32 +1653,32 @@
       <c r="C32" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="33">
         <v>43.7</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="33">
         <v>74.3</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="33">
         <v>65.5</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="39"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="18" t="s">
@@ -1680,18 +1687,18 @@
       <c r="C34" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="34">
+      <c r="D34" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="33">
         <v>81.599999999999994</v>
       </c>
-      <c r="F34" s="34" t="s">
-        <v>101</v>
+      <c r="F34" s="33" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="18" t="s">
@@ -1700,32 +1707,32 @@
       <c r="C35" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="34">
+      <c r="D35" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="33">
         <v>67.099999999999994</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="33">
         <v>59.3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="24" customFormat="1">
-      <c r="A36" s="26" t="s">
+    <row r="36" spans="1:6" s="23" customFormat="1">
+      <c r="A36" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B37" s="18" t="s">
@@ -1734,18 +1741,18 @@
       <c r="C37" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="33">
         <v>42.5</v>
       </c>
-      <c r="E37" s="34">
+      <c r="E37" s="33">
         <v>66.5</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="33">
         <v>48.9</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>83</v>
       </c>
       <c r="B38" s="18" t="s">
@@ -1754,18 +1761,18 @@
       <c r="C38" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="34">
+      <c r="D38" s="33">
         <v>37.799999999999997</v>
       </c>
-      <c r="E38" s="34">
+      <c r="E38" s="33">
         <v>60.7</v>
       </c>
-      <c r="F38" s="34">
+      <c r="F38" s="33">
         <v>58.2</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="18" t="s">
@@ -1774,18 +1781,18 @@
       <c r="C39" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="33">
         <v>39.1</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="33">
         <v>69.2</v>
       </c>
-      <c r="F39" s="34">
+      <c r="F39" s="33">
         <v>58.4</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>85</v>
       </c>
       <c r="B40" s="18" t="s">
@@ -1794,18 +1801,18 @@
       <c r="C40" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D40" s="34">
+      <c r="D40" s="33">
         <v>45.1</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="33">
         <v>69.3</v>
       </c>
-      <c r="F40" s="34">
+      <c r="F40" s="33">
         <v>62.2</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>86</v>
       </c>
       <c r="B41" s="19" t="s">
@@ -1814,25 +1821,25 @@
       <c r="C41" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="42">
         <v>45.3</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="42">
         <v>71.400000000000006</v>
       </c>
-      <c r="F41" s="43">
+      <c r="F41" s="42">
         <v>67.5</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="25.5" customHeight="1">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>107</v>
+      <c r="C42" s="47" t="s">
+        <v>111</v>
       </c>
       <c r="D42" s="20"/>
     </row>

</xml_diff>